<commit_message>
added logs for testing
</commit_message>
<xml_diff>
--- a/out/artifacts/vCheck1_1/12313123123.xlsx
+++ b/out/artifacts/vCheck1_1/12313123123.xlsx
@@ -2010,88 +2010,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B1BC44F1-0229-4768-9F52-A9155E5C8747}" diskRevisions="1" revisionId="27" version="2" preserveHistory="1825">
-  <header guid="{87E6FDFD-96EF-4286-BAB0-CE840E5BB314}" dateTime="2013-05-09T14:17:33" maxSheetId="4" userName="HPF-WS-02" r:id="rId1">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{92ED58A7-547D-43F9-A53A-E1DBCD9413CF}" dateTime="2013-05-09T14:20:29" maxSheetId="4" userName="HPF-WS-02" r:id="rId2" minRId="1">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{3284D0FD-EAB3-451D-A1EA-1F3996093AD3}" dateTime="2013-05-09T14:21:00" maxSheetId="4" userName="HPF-WS-02" r:id="rId3" minRId="2">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{6A8566BC-BEFC-4993-83CF-C26E96020A53}" dateTime="2013-05-09T14:22:07" maxSheetId="4" userName="HPF-WS-02" r:id="rId4" minRId="3" maxRId="4">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{46DB9F3D-406A-4254-95DE-45DFAE09C1D7}" dateTime="2013-05-09T14:25:28" maxSheetId="4" userName="Curt Franklin" r:id="rId5">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{4006E6F5-B5B6-4F9A-819F-A1B6CA35E69E}" dateTime="2013-05-09T14:25:59" maxSheetId="4" userName="Curt Franklin" r:id="rId6" minRId="5" maxRId="6">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D248C0D1-3374-4C24-8439-C5C338305024}" dateTime="2013-05-09T14:26:18" maxSheetId="4" userName="Curt Franklin" r:id="rId7">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{93BA7A30-01AA-4DA2-8D44-8764B57E57AA}" dateTime="2013-05-09T15:45:06" maxSheetId="4" userName="HPF-WS-02" r:id="rId8">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{97BA56BD-24AA-4D3B-B231-F88B4C6D364F}" dateTime="2013-05-09T15:51:02" maxSheetId="4" userName="HPF-WS-02" r:id="rId9" minRId="7" maxRId="26">
-    <sheetIdMap count="3">
-      <sheetId val="0"/>
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{7B051AFF-644B-4C77-A8FA-1AEAF75967F4}" dateTime="2013-05-09T16:03:06" maxSheetId="5" userName="Nicole VanDyke" r:id="rId10" minRId="27">
-    <sheetIdMap count="4">
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-      <sheetId val="65535"/>
-      <sheetId val="6911"/>
-    </sheetIdMap>
-    <reviewedList count="1">
-      <reviewed rId="27"/>
-    </reviewedList>
-  </header>
-  <header guid="{F6B53A00-50BB-4E43-834F-0A964A96FE66}" dateTime="2013-05-09T16:03:19" maxSheetId="5" userName="Nicole VanDyke" r:id="rId11">
-    <sheetIdMap count="4">
-      <sheetId val="32"/>
-      <sheetId val="0"/>
-      <sheetId val="65535"/>
-      <sheetId val="14848"/>
-    </sheetIdMap>
-  </header>
   <header guid="{38C3440D-4EC0-4292-BC84-4A302E87F478}" dateTime="2014-08-25T14:40:29" maxSheetId="5" userName="Nicole VanDyke" r:id="rId12">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -2127,24 +2045,6 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <ris rId="27" sheetId="4" name="[HPF-xxx Backend Volume Check Template.xls]Sheet1" sheetPosition="3"/>
-  <rcv guid="{9F84A064-4324-4DEF-94DB-E2DBDFD7C916}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{9F84A064-4324-4DEF-94DB-E2DBDFD7C916}" action="delete"/>
-  <rcv guid="{9F84A064-4324-4DEF-94DB-E2DBDFD7C916}" action="add"/>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{E305E553-7664-4FB6-A7EB-4038600BBB9A}" action="delete"/>
@@ -2174,254 +2074,10 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1" sId="1">
-    <nc r="B1" t="inlineStr">
-      <is>
-        <t>audit test</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="delete"/>
-  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="2" sId="1">
-    <oc r="B1" t="inlineStr">
-      <is>
-        <t>audit test</t>
-      </is>
-    </oc>
-    <nc r="B1"/>
-  </rcc>
-  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="delete"/>
-  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="3" sId="3">
-    <nc r="C27" t="inlineStr">
-      <is>
-        <t>Golda Monohon</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="4" sId="3" numFmtId="19">
-    <nc r="E27">
-      <v>41403</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{E305E553-7664-4FB6-A7EB-4038600BBB9A}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="5" sId="3">
-    <nc r="C29" t="inlineStr">
-      <is>
-        <t>Curt Franklin</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="6" sId="3" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E29">
-      <v>41403</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{E305E553-7664-4FB6-A7EB-4038600BBB9A}" action="delete"/>
-  <rcv guid="{E305E553-7664-4FB6-A7EB-4038600BBB9A}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="delete"/>
-  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="7" sId="3">
-    <nc r="E12" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8" sId="3">
-    <nc r="F12" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="9" sId="3">
-    <nc r="E13" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="10" sId="3">
-    <nc r="F13" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="11" sId="3">
-    <nc r="E14" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="12" sId="3">
-    <nc r="F14" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="13" sId="3">
-    <nc r="E15" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="14" sId="3">
-    <nc r="F15" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="15" sId="3">
-    <nc r="E16" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="3">
-    <nc r="F16" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="17" sId="3">
-    <nc r="E17" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="18" sId="3">
-    <nc r="F17" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="19" sId="3">
-    <nc r="E21" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="20" sId="3">
-    <nc r="F21" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="21" sId="3">
-    <nc r="E18" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="22" sId="3">
-    <nc r="F18" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="23" sId="3">
-    <nc r="E22" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="24" sId="3">
-    <nc r="F22" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="25" sId="3">
-    <nc r="E25" t="inlineStr">
-      <is>
-        <t>Pass</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="26" sId="3" odxf="1" dxf="1">
-    <nc r="F25" t="inlineStr">
-      <is>
-        <t>GLM  5/9/2013</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <b val="0"/>
-        <sz val="9"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-      </font>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{B1BC44F1-0229-4768-9F52-A9155E5C8747}" name="Microsoft Office User" id="-296995593" dateTime="2018-10-11T13:17:42"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
fixed bug with template merge method when the total number of well exceeds 96 (like invitae plates)
</commit_message>
<xml_diff>
--- a/out/artifacts/vCheck1_1/12313123123.xlsx
+++ b/out/artifacts/vCheck1_1/12313123123.xlsx
@@ -2075,9 +2075,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{B1BC44F1-0229-4768-9F52-A9155E5C8747}" name="Microsoft Office User" id="-296995593" dateTime="2018-10-11T13:17:42"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>